<commit_message>
Fixed courseDb type representation &add export xls
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -55,7 +55,7 @@
     <t>intro to fucking</t>
   </si>
   <si>
-    <t>L</t>
+    <t>lecture</t>
   </si>
   <si>
     <t>SHB</t>
@@ -109,13 +109,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -147,16 +147,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -475,17 +472,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="3.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="7.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="42.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="3.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="7.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="42.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -524,7 +521,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -559,7 +556,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -594,7 +591,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">

</xml_diff>

<commit_message>
field: department added to course schema
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Sem</t>
   </si>
@@ -25,6 +25,9 @@
     <t>CourseName</t>
   </si>
   <si>
+    <t>Department</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
   </si>
   <si>
     <t>intro to fucking</t>
+  </si>
+  <si>
+    <t>computer science</t>
   </si>
   <si>
     <t>L</t>
@@ -109,13 +115,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -147,16 +153,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -469,23 +472,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="3.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="7.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="42.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="3.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="7.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="42.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -501,19 +505,19 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -522,110 +526,122 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="3">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="3">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="3">
         <v>100</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="3">
+        <v>50</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="3">
-        <v>50</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>50</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished my course page
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boris/Desktop/CSCI3100/CUBRO/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DE0373-ADD7-5849-88BC-EC4BF548B291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>CourseCode</t>
   </si>
@@ -28,15 +34,9 @@
     <t>Instructor</t>
   </si>
   <si>
-    <t>Dates</t>
-  </si>
-  <si>
     <t>Seat</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Venue</t>
   </si>
   <si>
@@ -49,56 +49,59 @@
     <t>intro to fucking</t>
   </si>
   <si>
-    <t>computer science</t>
+    <t>Engineering</t>
   </si>
   <si>
     <t>KKL</t>
   </si>
   <si>
-    <t>2023-02-01,2023-02-02,2023-02-03,2023-02-08</t>
+    <t>SHB</t>
+  </si>
+  <si>
+    <t>dasdasdasda</t>
+  </si>
+  <si>
+    <t>EFGH5673</t>
+  </si>
+  <si>
+    <t>intro to puss</t>
+  </si>
+  <si>
+    <t>ALAN</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>EFGH5678</t>
+  </si>
+  <si>
+    <t>intro to dick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engineering
+</t>
+  </si>
+  <si>
+    <t>asdasdasd</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
   <si>
     <t>4-00-02,3-03-04</t>
   </si>
   <si>
-    <t>SHB</t>
-  </si>
-  <si>
-    <t>dasdasdasda</t>
-  </si>
-  <si>
-    <t>EFGH5673</t>
-  </si>
-  <si>
-    <t>intro to puss</t>
-  </si>
-  <si>
-    <t>ALAN</t>
-  </si>
-  <si>
-    <t>5-12-13</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>EFGH5678</t>
-  </si>
-  <si>
-    <t>intro to dick</t>
-  </si>
-  <si>
     <t>4-07-08</t>
   </si>
   <si>
-    <t>asdasdasd</t>
+    <t>5-11-12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,29 +144,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -174,10 +175,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -215,71 +216,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -307,7 +308,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -330,11 +331,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -343,13 +344,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -359,7 +360,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -368,7 +369,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -377,7 +378,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -385,10 +386,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -453,144 +454,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="24.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="7.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="7" max="8" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>100</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1">
+        <v>50</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2">
-        <v>100</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="E4" s="1">
+        <v>50</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2">
-        <v>50</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="H4" t="s">
         <v>20</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2">
-        <v>50</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix on course info
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boris/Desktop/CSCI3100/CUBRO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DE0373-ADD7-5849-88BC-EC4BF548B291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23F7DCC-05BA-3444-A51D-059010FB66ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>CourseCode</t>
   </si>
@@ -77,10 +77,6 @@
   </si>
   <si>
     <t>intro to dick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engineering
-</t>
   </si>
   <si>
     <t>asdasdasd</t>
@@ -144,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -153,6 +149,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +460,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -492,7 +491,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -518,7 +517,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -544,7 +543,7 @@
         <v>50</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -560,8 +559,8 @@
       <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -570,13 +569,13 @@
         <v>50</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>